<commit_message>
Committing Updated User feature file and corresponding actions calss and step definition class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_Request_Details.xlsx
+++ b/src/test/resources/TestData/LMS_Request_Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Testing\Saritha\Team14_REST-riders_Phase2_API_Hackathon_March_2025\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A25F1-8219-4903-BEAC-F96BC4DE35CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255B3511-4283-4051-8E24-A88EAE3298F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{3FD06A39-B92B-4AF5-883B-BAE6CEE67F63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3FD06A39-B92B-4AF5-883B-BAE6CEE67F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>invalidBatchId</t>
   </si>
   <si>
     <t>345678</t>
+  </si>
+  <si>
+    <t>invalidProgramId</t>
+  </si>
+  <si>
+    <t>209876</t>
   </si>
 </sst>
 </file>
@@ -418,23 +424,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC2856D-0E16-462E-B51B-999B4878E1AD}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C790C6B-05C4-4A50-97DB-A3FC8A5CA055}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
User Module Latest Code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_Request_Details.xlsx
+++ b/src/test/resources/TestData/LMS_Request_Details.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0FECEAC3-3E8F-438E-B188-773B4DA885B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{15D86632-76C4-4664-A4FE-1C8557B70E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3FD06A39-B92B-4AF5-883B-BAE6CEE67F63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{3FD06A39-B92B-4AF5-883B-BAE6CEE67F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N25"/>
+  <oleSize ref="A1:Q5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>invalidBatchId</t>
   </si>
@@ -34,6 +34,72 @@
   </si>
   <si>
     <t>userId</t>
+  </si>
+  <si>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>userEduPg</t>
+  </si>
+  <si>
+    <t>userEduUg</t>
+  </si>
+  <si>
+    <t>userFirstName</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userLinkedinUrl</t>
+  </si>
+  <si>
+    <t>userLocation</t>
+  </si>
+  <si>
+    <t>userMiddleName</t>
+  </si>
+  <si>
+    <t>userPhoneNumber</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userVisaStatus</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Ban</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sampl</t>
+  </si>
+  <si>
+    <t>US-Citizen</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>MBA</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>A60</t>
   </si>
   <si>
     <t>U50</t>
@@ -409,16 +475,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC2856D-0E16-462E-B51B-999B4878E1AD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>1234600789</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:13" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5CAC56-9F05-47F8-ABBE-85C6E0C468AB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -433,36 +608,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5CAC56-9F05-47F8-ABBE-85C6E0C468AB}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Committing Positive and negative scenarios of User module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_Request_Details.xlsx
+++ b/src/test/resources/TestData/LMS_Request_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Testing\Saritha\Team14_REST-riders_Phase2_API_Hackathon_March_2025\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255B3511-4283-4051-8E24-A88EAE3298F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6642E477-06DF-4D3A-B400-157068897D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3FD06A39-B92B-4AF5-883B-BAE6CEE67F63}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>invalidBatchId</t>
   </si>
@@ -52,16 +52,160 @@
   </si>
   <si>
     <t>209876</t>
+  </si>
+  <si>
+    <t>batchName</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>Team14-REST-riders</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>invalidRoleId</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LoginEmail</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>EDUPG</t>
+  </si>
+  <si>
+    <t>Saritha</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>Bsc</t>
+  </si>
+  <si>
+    <t>MCA</t>
+  </si>
+  <si>
+    <t>Ready to learn</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/1234</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>KSG</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>EDUUG</t>
+  </si>
+  <si>
+    <t>RoleId</t>
+  </si>
+  <si>
+    <t>RoleStatus</t>
+  </si>
+  <si>
+    <t>visaStatus</t>
+  </si>
+  <si>
+    <t>LinkedinUrl</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>Software  Development Engineer in Test</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>batchDesc</t>
+  </si>
+  <si>
+    <t>First Batch of SDET</t>
+  </si>
+  <si>
+    <t>batchNoOfClasses</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>9999999999</t>
+  </si>
+  <si>
+    <t>restriders_team14_punitha@gmail.com</t>
+  </si>
+  <si>
+    <t>Team14-REST-riders-SDET-31</t>
+  </si>
+  <si>
+    <t>SDET-002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,14 +228,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,47 +574,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC2856D-0E16-462E-B51B-999B4878E1AD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="34.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="V1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="V2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{7FEAB59C-EB42-4ED3-831E-9984CE172D9F}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{3334A0B5-1877-4C8D-A65C-A7A682FC5F03}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5CAC56-9F05-47F8-ABBE-85C6E0C468AB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Committing updated LMS api chaining codes with validations
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_Request_Details.xlsx
+++ b/src/test/resources/TestData/LMS_Request_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Testing\Saritha\Team14_REST-riders_Phase2_API_Hackathon_March_2025\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6642E477-06DF-4D3A-B400-157068897D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6991B7E-6819-4669-BBD2-9E00D9BDB915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3FD06A39-B92B-4AF5-883B-BAE6CEE67F63}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>invalidBatchId</t>
   </si>
@@ -93,15 +93,6 @@
     <t>EDUPG</t>
   </si>
   <si>
-    <t>Saritha</t>
-  </si>
-  <si>
-    <t>Gupta</t>
-  </si>
-  <si>
-    <t>R01</t>
-  </si>
-  <si>
     <t>CST</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>firstName</t>
   </si>
   <si>
-    <t>KSG</t>
-  </si>
-  <si>
     <t>lastName</t>
   </si>
   <si>
@@ -171,16 +159,40 @@
     <t>3</t>
   </si>
   <si>
-    <t>9999999999</t>
-  </si>
-  <si>
-    <t>restriders_team14_punitha@gmail.com</t>
-  </si>
-  <si>
-    <t>Team14-REST-riders-SDET-31</t>
-  </si>
-  <si>
-    <t>SDET-002</t>
+    <t>validProgId_User</t>
+  </si>
+  <si>
+    <t>16265</t>
+  </si>
+  <si>
+    <t>8470</t>
+  </si>
+  <si>
+    <t>validBatchId_User</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>SDET-007</t>
+  </si>
+  <si>
+    <t>LMSstaff</t>
+  </si>
+  <si>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>Teamfourteen</t>
+  </si>
+  <si>
+    <t>Team14-REST-riders-SDET-51</t>
+  </si>
+  <si>
+    <t>restriders_team14_Staff_j@gmail.com</t>
+  </si>
+  <si>
+    <t>5754525409</t>
   </si>
 </sst>
 </file>
@@ -574,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC2856D-0E16-462E-B51B-999B4878E1AD}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -597,38 +609,40 @@
     <col min="13" max="13" width="30.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="34.85546875" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" style="1" customWidth="1"/>
     <col min="20" max="20" width="13.140625" style="1" customWidth="1"/>
     <col min="21" max="21" width="16.42578125" style="1" customWidth="1"/>
     <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
     <col min="23" max="23" width="13" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="24" max="24" width="16.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>15</v>
@@ -637,16 +651,16 @@
         <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
@@ -658,16 +672,16 @@
         <v>13</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>0</v>
@@ -678,67 +692,73 @@
       <c r="W1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>1</v>
@@ -748,6 +768,12 @@
       </c>
       <c r="W2" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>